<commit_message>
update to the latest version by LIu mingjing
</commit_message>
<xml_diff>
--- a/doc/APfollowup.xlsx
+++ b/doc/APfollowup.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>项目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -66,6 +66,18 @@
   </si>
   <si>
     <t>目前为止，看到一个比较好的网站：高考派，该网站做这个内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>准备思维导图，想想处理逻辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>先从杭州做起：浙江省高考政策，高考学生数据，高考学生人数，坐落于杭州的大学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>先做微信版本，APP先放放。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -109,8 +121,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,22 +406,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="65.625" customWidth="1"/>
+    <col min="2" max="2" width="65.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -420,7 +435,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
@@ -431,7 +446,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
@@ -442,7 +457,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -450,7 +465,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
@@ -461,16 +476,35 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>